<commit_message>
updated spreadsheets for summary of metrics for pkis1 loto and p-values
</commit_message>
<xml_diff>
--- a/output_pkis1loto/metrics/pkis1loto_eval_all_metrics.xlsx
+++ b/output_pkis1loto/metrics/pkis1loto_eval_all_metrics.xlsx
@@ -943,8 +943,8 @@
   </sheetPr>
   <dimension ref="A2:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1635,7 +1635,7 @@
   <dimension ref="A1:U225"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="1" sqref="A17:K25 L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9010,7 +9010,7 @@
   <dimension ref="A1:U225"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="1" sqref="A17:K25 L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16385,7 +16385,7 @@
   <dimension ref="A1:U225"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="1" sqref="A17:K25 L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23759,13 +23759,13 @@
   <dimension ref="A1:U225"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="1" sqref="A17:K25 L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="4" width="6.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="4" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="13" style="0" width="5.55"/>
@@ -31134,12 +31134,12 @@
   <dimension ref="A1:U225"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="1" sqref="A17:K25 L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="4" width="6.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="13" style="0" width="5.55"/>

</xml_diff>

<commit_message>
updated shebang in python scripts to match general environment: '/usr/bin/env python2'
</commit_message>
<xml_diff>
--- a/output_pkis1loto/metrics/pkis1loto_eval_all_metrics.xlsx
+++ b/output_pkis1loto/metrics/pkis1loto_eval_all_metrics.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="pkis1loto_eval_ROCAUC_v1.2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="pkis1loto_eval_NEF10_v1.2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="pkis1loto_eval_FASR10_v1.2" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="pkis1loto_eval_ROCAUC" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="pkis1loto_eval_NEF10" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="pkis1loto_eval_FASR10" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="PKIS1LOTO MCC" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="PKIS1LOTO F1" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="summary_MCC_F1_thresholding" sheetId="7" state="visible" r:id="rId8"/>
@@ -960,7 +960,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1034,10 +1034,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1172,7 +1168,7 @@
   </sheetPr>
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -24158,8 +24154,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="18.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="18.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="5" width="5.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="2.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="13" style="5" width="5.81"/>
@@ -24481,7 +24477,7 @@
       <c r="AO3" s="5" t="n">
         <v>0.929291920503345</v>
       </c>
-      <c r="AQ3" s="19" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>249</v>
       </c>
       <c r="AR3" s="5" t="n">
@@ -24785,7 +24781,7 @@
       <c r="AO5" s="5" t="n">
         <v>0.911668887178053</v>
       </c>
-      <c r="AQ5" s="20" t="s">
+      <c r="AQ5" s="19" t="s">
         <v>251</v>
       </c>
       <c r="AR5" s="5" t="n">
@@ -26226,18 +26222,18 @@
       <c r="AO16" s="5" t="n">
         <v>0.660096921891062</v>
       </c>
-      <c r="AQ16" s="21" t="s">
+      <c r="AQ16" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="AR16" s="22"/>
-      <c r="AS16" s="22"/>
-      <c r="AT16" s="22"/>
-      <c r="AU16" s="22"/>
-      <c r="AV16" s="22"/>
-      <c r="AW16" s="22"/>
-      <c r="AX16" s="22"/>
-      <c r="AY16" s="22"/>
-      <c r="AZ16" s="23"/>
+      <c r="AR16" s="21"/>
+      <c r="AS16" s="21"/>
+      <c r="AT16" s="21"/>
+      <c r="AU16" s="21"/>
+      <c r="AV16" s="21"/>
+      <c r="AW16" s="21"/>
+      <c r="AX16" s="21"/>
+      <c r="AY16" s="21"/>
+      <c r="AZ16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
@@ -26351,7 +26347,7 @@
       <c r="AO17" s="5" t="n">
         <v>0.472296650328152</v>
       </c>
-      <c r="AQ17" s="24" t="s">
+      <c r="AQ17" s="23" t="s">
         <v>251</v>
       </c>
       <c r="AR17" s="18" t="s">
@@ -26378,7 +26374,7 @@
       <c r="AY17" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="AZ17" s="25" t="s">
+      <c r="AZ17" s="24" t="s">
         <v>8</v>
       </c>
     </row>
@@ -26494,7 +26490,7 @@
       <c r="AO18" s="5" t="n">
         <v>0.560384123517674</v>
       </c>
-      <c r="AQ18" s="26" t="s">
+      <c r="AQ18" s="25" t="s">
         <v>10</v>
       </c>
       <c r="AR18" s="5" t="n">
@@ -26529,7 +26525,7 @@
         <f aca="false">AVERAGE(AN3:AN226)</f>
         <v>0.48052124694332</v>
       </c>
-      <c r="AZ18" s="27" t="n">
+      <c r="AZ18" s="26" t="n">
         <f aca="false">AVERAGE(AO3:AO226)</f>
         <v>0.542322810669355</v>
       </c>
@@ -26646,7 +26642,7 @@
       <c r="AO19" s="5" t="n">
         <v>0.264210086694489</v>
       </c>
-      <c r="AQ19" s="26" t="s">
+      <c r="AQ19" s="25" t="s">
         <v>11</v>
       </c>
       <c r="AR19" s="5" t="n">
@@ -26681,7 +26677,7 @@
         <f aca="false">MEDIAN(AN3:AN226)</f>
         <v>0.483133375069748</v>
       </c>
-      <c r="AZ19" s="27" t="n">
+      <c r="AZ19" s="26" t="n">
         <f aca="false">MEDIAN(AO3:AO226)</f>
         <v>0.554627645141132</v>
       </c>
@@ -26798,42 +26794,42 @@
       <c r="AO20" s="5" t="n">
         <v>0.236560497218586</v>
       </c>
-      <c r="AQ20" s="28" t="s">
+      <c r="AQ20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AR20" s="29" t="n">
+      <c r="AR20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AG3:AG226)</f>
         <v>0.20075757682535</v>
       </c>
-      <c r="AS20" s="29" t="n">
+      <c r="AS20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AH3:AH226)</f>
         <v>0.195391220783512</v>
       </c>
-      <c r="AT20" s="29" t="n">
+      <c r="AT20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AI3:AI226)</f>
         <v>0.210419526480984</v>
       </c>
-      <c r="AU20" s="29" t="n">
+      <c r="AU20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AJ3:AJ226)</f>
         <v>0.191509604424979</v>
       </c>
-      <c r="AV20" s="29" t="n">
+      <c r="AV20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AK3:AK226)</f>
         <v>0.196111984420009</v>
       </c>
-      <c r="AW20" s="29" t="n">
+      <c r="AW20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AL3:AL226)</f>
         <v>0.200695970135256</v>
       </c>
-      <c r="AX20" s="29" t="n">
+      <c r="AX20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AM3:AM226)</f>
         <v>0.21538800975023</v>
       </c>
-      <c r="AY20" s="29" t="n">
+      <c r="AY20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AN3:AN226)</f>
         <v>0.236567692300584</v>
       </c>
-      <c r="AZ20" s="30" t="n">
+      <c r="AZ20" s="29" t="n">
         <f aca="false">_xlfn.STDEV.P(AO3:AO226)</f>
         <v>0.229660716078704</v>
       </c>
@@ -50156,16 +50152,16 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="W1" s="31" t="s">
+      <c r="W1" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="AG1" s="31" t="s">
+      <c r="AG1" s="30" t="s">
         <v>254</v>
       </c>
       <c r="AQ1" s="17" t="s">
@@ -50311,7 +50307,7 @@
       <c r="AO2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AQ2" s="19" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>248</v>
       </c>
       <c r="AR2" s="5" t="n">
@@ -50463,7 +50459,7 @@
       <c r="AO3" s="5" t="n">
         <v>0.935483870967742</v>
       </c>
-      <c r="AQ3" s="19" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>249</v>
       </c>
       <c r="AR3" s="5" t="n">
@@ -50615,7 +50611,7 @@
       <c r="AO4" s="5" t="n">
         <v>0.950819672131148</v>
       </c>
-      <c r="AQ4" s="19" t="s">
+      <c r="AQ4" s="2" t="s">
         <v>250</v>
       </c>
       <c r="AR4" s="5" t="n">
@@ -50767,7 +50763,7 @@
       <c r="AO5" s="5" t="n">
         <v>0.918032786885246</v>
       </c>
-      <c r="AQ5" s="20" t="s">
+      <c r="AQ5" s="19" t="s">
         <v>251</v>
       </c>
       <c r="AR5" s="5" t="n">
@@ -52199,18 +52195,18 @@
       <c r="AO16" s="5" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="AQ16" s="21" t="s">
+      <c r="AQ16" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="AR16" s="22"/>
-      <c r="AS16" s="22"/>
-      <c r="AT16" s="22"/>
-      <c r="AU16" s="22"/>
-      <c r="AV16" s="22"/>
-      <c r="AW16" s="22"/>
-      <c r="AX16" s="22"/>
-      <c r="AY16" s="22"/>
-      <c r="AZ16" s="23"/>
+      <c r="AR16" s="21"/>
+      <c r="AS16" s="21"/>
+      <c r="AT16" s="21"/>
+      <c r="AU16" s="21"/>
+      <c r="AV16" s="21"/>
+      <c r="AW16" s="21"/>
+      <c r="AX16" s="21"/>
+      <c r="AY16" s="21"/>
+      <c r="AZ16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -52324,7 +52320,7 @@
       <c r="AO17" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="AQ17" s="24" t="s">
+      <c r="AQ17" s="23" t="s">
         <v>251</v>
       </c>
       <c r="AR17" s="18" t="s">
@@ -52351,7 +52347,7 @@
       <c r="AY17" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="AZ17" s="25" t="s">
+      <c r="AZ17" s="24" t="s">
         <v>8</v>
       </c>
     </row>
@@ -52467,7 +52463,7 @@
       <c r="AO18" s="5" t="n">
         <v>0.585365853658537</v>
       </c>
-      <c r="AQ18" s="26" t="s">
+      <c r="AQ18" s="25" t="s">
         <v>10</v>
       </c>
       <c r="AR18" s="5" t="n">
@@ -52502,7 +52498,7 @@
         <f aca="false">AVERAGE(AN3:AN226)</f>
         <v>0.499873311402425</v>
       </c>
-      <c r="AZ18" s="27" t="n">
+      <c r="AZ18" s="26" t="n">
         <f aca="false">AVERAGE(AO3:AO226)</f>
         <v>0.557566516467118</v>
       </c>
@@ -52619,7 +52615,7 @@
       <c r="AO19" s="5" t="n">
         <v>0.307692307692308</v>
       </c>
-      <c r="AQ19" s="26" t="s">
+      <c r="AQ19" s="25" t="s">
         <v>11</v>
       </c>
       <c r="AR19" s="5" t="n">
@@ -52654,7 +52650,7 @@
         <f aca="false">MEDIAN(AN3:AN226)</f>
         <v>0.5</v>
       </c>
-      <c r="AZ19" s="27" t="n">
+      <c r="AZ19" s="26" t="n">
         <f aca="false">MEDIAN(AO3:AO226)</f>
         <v>0.563492063492063</v>
       </c>
@@ -52771,42 +52767,42 @@
       <c r="AO20" s="5" t="n">
         <v>0.285714285714286</v>
       </c>
-      <c r="AQ20" s="28" t="s">
+      <c r="AQ20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AR20" s="29" t="n">
+      <c r="AR20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AG3:AG226)</f>
         <v>0.188866585585266</v>
       </c>
-      <c r="AS20" s="29" t="n">
+      <c r="AS20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AH3:AH226)</f>
         <v>0.183832561101638</v>
       </c>
-      <c r="AT20" s="29" t="n">
+      <c r="AT20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AI3:AI226)</f>
         <v>0.19759937406274</v>
       </c>
-      <c r="AU20" s="29" t="n">
+      <c r="AU20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AJ3:AJ226)</f>
         <v>0.17734206655758</v>
       </c>
-      <c r="AV20" s="29" t="n">
+      <c r="AV20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AK3:AK226)</f>
         <v>0.182319442743187</v>
       </c>
-      <c r="AW20" s="29" t="n">
+      <c r="AW20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AL3:AL226)</f>
         <v>0.186100564164812</v>
       </c>
-      <c r="AX20" s="29" t="n">
+      <c r="AX20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AM3:AM226)</f>
         <v>0.204082689202986</v>
       </c>
-      <c r="AY20" s="29" t="n">
+      <c r="AY20" s="28" t="n">
         <f aca="false">_xlfn.STDEV.P(AN3:AN226)</f>
         <v>0.224056316467074</v>
       </c>
-      <c r="AZ20" s="30" t="n">
+      <c r="AZ20" s="29" t="n">
         <f aca="false">_xlfn.STDEV.P(AO3:AO226)</f>
         <v>0.2202908433495</v>
       </c>
@@ -76107,7 +76103,7 @@
   </sheetPr>
   <dimension ref="A2:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -76223,7 +76219,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="15"/>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="2" t="s">
         <v>249</v>
       </c>
       <c r="D5" s="15"/>
@@ -76259,7 +76255,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="15"/>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="2" t="s">
         <v>250</v>
       </c>
       <c r="D6" s="15"/>
@@ -76295,7 +76291,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="15"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>251</v>
       </c>
       <c r="D7" s="15"/>
@@ -76331,7 +76327,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="15"/>
-      <c r="C8" s="19"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="15"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -76349,7 +76345,7 @@
       <c r="B9" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="2" t="s">
         <v>248</v>
       </c>
       <c r="D9" s="15"/>
@@ -76385,7 +76381,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="15"/>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="2" t="s">
         <v>249</v>
       </c>
       <c r="D10" s="15"/>
@@ -76457,7 +76453,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="15"/>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>251</v>
       </c>
       <c r="D12" s="15"/>

</xml_diff>